<commit_message>
Aggiunto collegamento a coverage index (generato con simplecov) su README.md e aggiornato TestCoverage basato su completamento features
</commit_message>
<xml_diff>
--- a/doc/documentation sources/TestCoverage.xlsx
+++ b/doc/documentation sources/TestCoverage.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gionni_2\Desktop\Università\UniTn\Didattica2017-18\IS2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,28 +57,6 @@
     <t>Coverage</t>
   </si>
   <si>
-    <t>Feature: A customer insert a new issue
-  Scenario: Entering a valid issue
-  Scenario: Entering an invalid issue</t>
-  </si>
-  <si>
-    <t>Feature: Inserting a new customer
-  Scenario: Entering valid information of a customer
-  Scenario: Entering incomplete information of a customer</t>
-  </si>
-  <si>
-    <t>Feature: Service for a customer
-  Scenario: Start the timer
-  Scenario: Stop the time
-  Scenario: Incomplete data
-  Scenario: Complete data</t>
-  </si>
-  <si>
-    <t>Feature: invoice for a customer
-  Scenario: Entering valid information of a invoice
-  Scenario: Issue the invoice</t>
-  </si>
-  <si>
     <t xml:space="preserve">Feature: Search a customer
   Scenario: Entering a filter string    </t>
   </si>
@@ -102,12 +75,38 @@
   <si>
     <t>Skipped</t>
   </si>
+  <si>
+    <t>Feature: Inserting a new customer
+  Scenario: Entering valid information of a customer
+  Scenario: Entering incomplete information of a customer
+Feature: Update and delete customer
+  Scenario: Valid update to a customer
+  Scenario: Invalid update to a customer
+  Scenario: Delete a customer</t>
+  </si>
+  <si>
+    <t>Feature: Service for a customer
+  Scenario: Incomplete data
+  Scenario: Complete data</t>
+  </si>
+  <si>
+    <t>Feature: A customer insert a new issue
+  Scenario: Entering a valid issue
+  Scenario: Entering an invalid issue
+Feature: Managing issues
+  Scenario: New issue</t>
+  </si>
+  <si>
+    <t>Feature: invoice for a customer
+  Scenario: Entering valid information of a invoice
+  Scenario: Pay the invoice</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +169,13 @@
     <font>
       <b/>
       <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -296,9 +302,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -332,6 +335,9 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,7 +358,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -385,7 +391,7 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
             <a:ln w="19050">
               <a:solidFill>
@@ -402,7 +408,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,7 +452,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -471,17 +477,6 @@
             <c:idx val="0"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-              <a:ln w="19050">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
@@ -506,11 +501,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="3911408"/>
-        <c:axId val="3910848"/>
+        <c:axId val="161454720"/>
+        <c:axId val="161143808"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="3910848"/>
+        <c:axId val="161143808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,12 +529,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3911408"/>
+        <c:crossAx val="161454720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="3911408"/>
+        <c:axId val="161454720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -549,7 +544,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="3910848"/>
+        <c:crossAx val="161143808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -604,7 +599,7 @@
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -654,7 +649,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -710,7 +705,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,7 +733,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -754,11 +749,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="162582672"/>
-        <c:axId val="162422544"/>
+        <c:axId val="102984704"/>
+        <c:axId val="102983168"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="162422544"/>
+        <c:axId val="102983168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -782,12 +777,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162582672"/>
+        <c:crossAx val="102984704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="162582672"/>
+        <c:axId val="102984704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162422544"/>
+        <c:crossAx val="102983168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -852,7 +847,7 @@
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -902,7 +897,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +953,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -986,7 +981,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1002,11 +997,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="162587152"/>
-        <c:axId val="162586592"/>
+        <c:axId val="103033088"/>
+        <c:axId val="103031552"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="162586592"/>
+        <c:axId val="103031552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,12 +1025,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162587152"/>
+        <c:crossAx val="103033088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="162587152"/>
+        <c:axId val="103033088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1040,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162586592"/>
+        <c:crossAx val="103031552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1100,7 +1095,7 @@
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1150,7 +1145,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1206,7 +1201,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1250,11 +1245,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="163272768"/>
-        <c:axId val="163272208"/>
+        <c:axId val="103065088"/>
+        <c:axId val="103063552"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="163272208"/>
+        <c:axId val="103063552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1278,12 +1273,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163272768"/>
+        <c:crossAx val="103065088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="163272768"/>
+        <c:axId val="103065088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1288,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="163272208"/>
+        <c:crossAx val="103063552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1348,7 +1343,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1399,26 +1394,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
@@ -1426,6 +1401,7 @@
       <c:rotY val="0"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -1624,13 +1600,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1748,7 +1724,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1803,7 +1779,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1875,11 +1851,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="161849520"/>
-        <c:axId val="161848960"/>
+        <c:axId val="99911552"/>
+        <c:axId val="99910016"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="161848960"/>
+        <c:axId val="99910016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,12 +1879,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161849520"/>
+        <c:crossAx val="99911552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="161849520"/>
+        <c:axId val="99911552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,7 +1894,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161848960"/>
+        <c:crossAx val="99910016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1973,7 +1949,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2023,7 +1999,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2079,7 +2055,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2095,11 +2071,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="162278016"/>
-        <c:axId val="162277456"/>
+        <c:axId val="99932032"/>
+        <c:axId val="99930496"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="162277456"/>
+        <c:axId val="99930496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2123,12 +2099,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162278016"/>
+        <c:crossAx val="99932032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="162278016"/>
+        <c:axId val="99932032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2138,7 +2114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162277456"/>
+        <c:crossAx val="99930496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2193,7 +2169,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2243,7 +2219,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2299,7 +2275,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2315,11 +2291,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="162281936"/>
-        <c:axId val="162281376"/>
+        <c:axId val="100417920"/>
+        <c:axId val="99940992"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="162281376"/>
+        <c:axId val="99940992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,12 +2319,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162281936"/>
+        <c:crossAx val="100417920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="162281936"/>
+        <c:axId val="100417920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2358,7 +2334,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162281376"/>
+        <c:crossAx val="99940992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2413,7 +2389,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2463,7 +2439,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2519,7 +2495,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2535,11 +2511,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="162673616"/>
-        <c:axId val="162673056"/>
+        <c:axId val="100441088"/>
+        <c:axId val="100439552"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="162673056"/>
+        <c:axId val="100439552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,12 +2539,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162673616"/>
+        <c:crossAx val="100441088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="162673616"/>
+        <c:axId val="100441088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2578,7 +2554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162673056"/>
+        <c:crossAx val="100439552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2633,7 +2609,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2683,7 +2659,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2711,7 +2687,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2767,7 +2743,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2783,11 +2759,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="162678096"/>
-        <c:axId val="162677536"/>
+        <c:axId val="100493568"/>
+        <c:axId val="100492032"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="162677536"/>
+        <c:axId val="100492032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2811,12 +2787,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162678096"/>
+        <c:crossAx val="100493568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="162678096"/>
+        <c:axId val="100493568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2826,7 +2802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162677536"/>
+        <c:crossAx val="100492032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2881,7 +2857,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2932,26 +2908,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
@@ -2959,6 +2915,7 @@
       <c:rotY val="0"/>
       <c:depthPercent val="100"/>
       <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -3180,16 +3137,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3307,7 +3264,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3357,7 +3314,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3457,11 +3414,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="100"/>
-        <c:axId val="162418624"/>
-        <c:axId val="162418064"/>
+        <c:axId val="102963072"/>
+        <c:axId val="102961536"/>
       </c:barChart>
       <c:valAx>
-        <c:axId val="162418064"/>
+        <c:axId val="102961536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3485,12 +3442,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162418624"/>
+        <c:crossAx val="102963072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="162418624"/>
+        <c:axId val="102963072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3500,7 +3457,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162418064"/>
+        <c:crossAx val="102961536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10555,13 +10512,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>226214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>981076</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>952499</xdr:rowOff>
+      <xdr:rowOff>1131089</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10747,13 +10704,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:rowOff>226214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>981076</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>952499</xdr:rowOff>
+      <xdr:rowOff>1131089</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11128,7 +11085,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11141,8 +11098,8 @@
   </sheetPr>
   <dimension ref="B2:O16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11161,136 +11118,136 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
     </row>
     <row r="3" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="23" t="s">
-        <v>18</v>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="22" t="s">
+        <v>14</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
     </row>
     <row r="5" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
     </row>
     <row r="6" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
     </row>
     <row r="7" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
     </row>
     <row r="8" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -11303,7 +11260,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>8</v>
@@ -11318,7 +11275,7 @@
         <v>11</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>8</v>
@@ -11329,8 +11286,8 @@
       <c r="M10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="21" t="s">
-        <v>21</v>
+      <c r="N10" s="20" t="s">
+        <v>17</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>11</v>
@@ -11340,44 +11297,44 @@
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E11" s="5">
         <f>SUM(E12:E105)</f>
-        <v>11</v>
+        <v>13</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="15">
         <f t="shared" ref="F11:H11" si="0">SUM(F12:F105)</f>
-        <v>2</v>
+        <v>13</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5">
         <f>SUM(J12:J105)</f>
-        <v>41</v>
+        <v>62</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="15">
         <f t="shared" ref="K11:L11" si="1">SUM(K12:K105)</f>
-        <v>12</v>
+        <v>62</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="13">
         <f>SUM(M12:M105)</f>
-        <v>10</v>
+        <v>0</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="21">
         <f>SUM(N12:N105)</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="O11" s="5"/>
     </row>
@@ -11388,82 +11345,86 @@
       <c r="C12" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>12</v>
+      <c r="D12" s="23" t="s">
+        <v>20</v>
       </c>
-      <c r="E12" s="17">
-        <v>2</v>
+      <c r="E12" s="16">
+        <f>2+1</f>
+        <v>3</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
+        <v>3</v>
+      </c>
+      <c r="G12" s="12">
         <v>0</v>
       </c>
-      <c r="G12" s="13">
-        <v>2</v>
-      </c>
-      <c r="H12" s="13">
+      <c r="H12" s="12">
         <f>E12-F12-G12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="17">
-        <v>8</v>
+      <c r="I12" s="11"/>
+      <c r="J12" s="16">
+        <f>10+5</f>
+        <v>15</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="12">
+        <v>15</v>
+      </c>
+      <c r="L12" s="12">
         <v>0</v>
       </c>
-      <c r="L12" s="13">
-        <v>2</v>
-      </c>
-      <c r="M12" s="13">
+      <c r="M12" s="12">
         <f t="shared" ref="M12:M13" si="2">J12-K12-L12-N12</f>
         <v>0</v>
       </c>
-      <c r="N12" s="13">
-        <v>6</v>
+      <c r="N12" s="12">
+        <v>0</v>
       </c>
-      <c r="O12" s="12"/>
+      <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="2:15" s="1" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" s="1" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>13</v>
+      <c r="D13" s="23" t="s">
+        <v>18</v>
       </c>
-      <c r="E13" s="17">
-        <v>2</v>
+      <c r="E13" s="16">
+        <f>2+3</f>
+        <v>5</v>
       </c>
-      <c r="F13" s="13">
-        <v>2</v>
+      <c r="F13" s="12">
+        <v>5</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>0</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <f>E13-F13-G13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="17">
-        <v>9</v>
+      <c r="I13" s="11"/>
+      <c r="J13" s="16">
+        <f>9+11</f>
+        <v>20</v>
       </c>
-      <c r="K13" s="13">
-        <v>9</v>
+      <c r="K13" s="12">
+        <v>20</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="12">
         <v>0</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="12">
         <v>0</v>
       </c>
-      <c r="O13" s="12"/>
+      <c r="O13" s="11"/>
     </row>
     <row r="14" spans="2:15" s="1" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
@@ -11472,40 +11433,40 @@
       <c r="C14" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>14</v>
+      <c r="D14" s="23" t="s">
+        <v>19</v>
       </c>
-      <c r="E14" s="17">
-        <v>4</v>
+      <c r="E14" s="16">
+        <v>2</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
+        <v>2</v>
+      </c>
+      <c r="G14" s="12">
         <v>0</v>
       </c>
-      <c r="G14" s="13">
+      <c r="H14" s="12">
+        <f>E14-F14-G14</f>
         <v>0</v>
       </c>
-      <c r="H14" s="13">
-        <f>E14-F14-G14</f>
-        <v>4</v>
+      <c r="I14" s="11"/>
+      <c r="J14" s="16">
+        <v>12</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="17">
-        <v>13</v>
+      <c r="K14" s="12">
+        <v>12</v>
       </c>
-      <c r="K14" s="13">
+      <c r="L14" s="12">
         <v>0</v>
       </c>
-      <c r="L14" s="13">
+      <c r="M14" s="12">
+        <f>J14-K14-L14-N14</f>
         <v>0</v>
       </c>
-      <c r="M14" s="13">
-        <f>J14-K14-L14-N14</f>
-        <v>4</v>
+      <c r="N14" s="12">
+        <v>0</v>
       </c>
-      <c r="N14" s="13">
-        <v>9</v>
-      </c>
-      <c r="O14" s="12"/>
+      <c r="O14" s="11"/>
     </row>
     <row r="15" spans="2:15" s="1" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9">
@@ -11514,40 +11475,40 @@
       <c r="C15" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>15</v>
+      <c r="D15" s="23" t="s">
+        <v>21</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="16">
         <v>2</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="12">
+        <v>2</v>
+      </c>
+      <c r="G15" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="13">
+      <c r="H15" s="12">
+        <f>E15-F15-G15</f>
         <v>0</v>
       </c>
-      <c r="H15" s="13">
-        <f>E15-F15-G15</f>
-        <v>2</v>
+      <c r="I15" s="11"/>
+      <c r="J15" s="16">
+        <v>11</v>
       </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="17">
-        <v>7</v>
+      <c r="K15" s="12">
+        <v>11</v>
       </c>
-      <c r="K15" s="13">
+      <c r="L15" s="12">
         <v>0</v>
       </c>
-      <c r="L15" s="13">
+      <c r="M15" s="12">
+        <f t="shared" ref="M15:M16" si="3">J15-K15-L15-N15</f>
         <v>0</v>
       </c>
-      <c r="M15" s="13">
-        <f t="shared" ref="M15:M16" si="3">J15-K15-L15-N15</f>
-        <v>5</v>
+      <c r="N15" s="12">
+        <v>0</v>
       </c>
-      <c r="N15" s="13">
-        <v>2</v>
-      </c>
-      <c r="O15" s="12"/>
+      <c r="O15" s="11"/>
     </row>
     <row r="16" spans="2:15" s="1" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
@@ -11556,40 +11517,40 @@
       <c r="C16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>16</v>
+      <c r="D16" s="23" t="s">
+        <v>12</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>1</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12">
         <v>0</v>
       </c>
-      <c r="G16" s="13">
+      <c r="H16" s="12">
+        <f>E16-F16-G16</f>
         <v>0</v>
       </c>
-      <c r="H16" s="13">
-        <f>E16-F16-G16</f>
-        <v>1</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="17">
+      <c r="I16" s="11"/>
+      <c r="J16" s="16">
         <v>4</v>
       </c>
-      <c r="K16" s="13">
-        <v>3</v>
+      <c r="K16" s="12">
+        <v>4</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="12">
         <v>0</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="12">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N16" s="13">
         <v>0</v>
       </c>
-      <c r="O16" s="12"/>
+      <c r="N16" s="12">
+        <v>0</v>
+      </c>
+      <c r="O16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>